<commit_message>
Automação da pesquisa pela lupa
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.oliveira\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.oliveira\git\hub-tdd\hub_tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C74EB1A-3311-4BB9-8B94-8984ABFA9334}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B6C08-489B-41AD-BF41-2864C4F622C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
+    <sheet name="Pesquisa pagina inicial" sheetId="2" r:id="rId2"/>
+    <sheet name="Pesquisa pela lupa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>login</t>
   </si>
@@ -69,9 +71,6 @@
     <t>cep</t>
   </si>
   <si>
-    <t>CaiqueOliveira</t>
-  </si>
-  <si>
     <t>Caique1</t>
   </si>
   <si>
@@ -100,6 +99,12 @@
   </si>
   <si>
     <t>caique@email.com</t>
+  </si>
+  <si>
+    <t>joaopedro</t>
+  </si>
+  <si>
+    <t>HP PAVILION 15Z TOUCH LAPTOP</t>
   </si>
 </sst>
 </file>
@@ -473,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECC51B8-0D12-4ED7-B203-D3656A8C93F0}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,40 +536,40 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -577,4 +582,35 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141451B3-9CBA-429A-9675-639952A6C031}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5326D1A-0578-42FA-82E8-01F57604A91B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Teste possitivo de login
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
@@ -3,21 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.oliveira\git\hub-tdd\hub_tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B6C08-489B-41AD-BF41-2864C4F622C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F455B794-27EA-4F88-9381-91C7BE603FC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
     <sheet name="Pesquisa pagina inicial" sheetId="2" r:id="rId2"/>
     <sheet name="Pesquisa pela lupa" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -478,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECC51B8-0D12-4ED7-B203-D3656A8C93F0}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -600,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5326D1A-0578-42FA-82E8-01F57604A91B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Foi implementados os reports nos testes
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.oliveira\git\ProjetoHub_TDD\projetoHub_tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54113BFD-D869-46E6-9869-20341C3CB3BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662FAE81-0D6C-47CD-B116-61BA6B673BB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="360" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>login</t>
   </si>
@@ -92,26 +92,29 @@
     <t>06462-090</t>
   </si>
   <si>
+    <t>HP PAVILION 15Z TOUCH LAPTOP</t>
+  </si>
+  <si>
+    <t>produto</t>
+  </si>
+  <si>
     <t>caique@email.com</t>
   </si>
   <si>
-    <t>HP PAVILION 15Z TOUCH LAPTOP</t>
-  </si>
-  <si>
-    <t>cauasantana</t>
-  </si>
-  <si>
-    <t>produto</t>
-  </si>
-  <si>
-    <t>HP Stream - 11-d020nr Laptop</t>
+    <t>Mouse óptico USB com 3 botões HP</t>
+  </si>
+  <si>
+    <t>HP ZBook 17 G2 Mobile Workstation</t>
+  </si>
+  <si>
+    <t>caiquasantanadeoliveira</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,9 +139,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF2A2A2A"/>
-      <name val="LocalRobotoRegular"/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,13 +173,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -490,7 +500,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -504,7 +514,7 @@
     <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,12 +552,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -580,7 +590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5" s="2"/>
     </row>
   </sheetData>
@@ -594,25 +604,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141451B3-9CBA-429A-9675-639952A6C031}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -627,11 +642,11 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Busca pela lupa falha terminado.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.oliveira\git\ProjetoHub_TDD\projetoHub_tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662FAE81-0D6C-47CD-B116-61BA6B673BB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB5E8B4-8E5C-4155-A5E0-AC0D0FDEC3CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>06462-090</t>
   </si>
   <si>
-    <t>HP PAVILION 15Z TOUCH LAPTOP</t>
-  </si>
-  <si>
     <t>produto</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>caiquasantanadeoliveira</t>
+  </si>
+  <si>
+    <t>HP ZBOOK 17 G2 MOBILE WORKSTATION</t>
   </si>
 </sst>
 </file>
@@ -554,10 +554,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -606,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141451B3-9CBA-429A-9675-639952A6C031}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -617,17 +617,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -640,13 +640,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5326D1A-0578-42FA-82E8-01F57604A91B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>21</v>
+      <c r="A1" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>